<commit_message>
Add species status: Fratercula arctica -> False Positive
</commit_message>
<xml_diff>
--- a/UK_Birds_Generalized_Status.xlsx
+++ b/UK_Birds_Generalized_Status.xlsx
@@ -474,7 +474,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C645"/>
+  <dimension ref="A1:C646"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
@@ -11451,6 +11451,23 @@
         </is>
       </c>
     </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>Atlantic Puffin</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>Fratercula arctica</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>False Positive</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Add species status: Fratercula arctica -> Summer visitor
</commit_message>
<xml_diff>
--- a/UK_Birds_Generalized_Status.xlsx
+++ b/UK_Birds_Generalized_Status.xlsx
@@ -474,7 +474,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C646"/>
+  <dimension ref="A1:C647"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
@@ -11468,6 +11468,23 @@
         </is>
       </c>
     </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>Atlantic Puffin</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Fratercula arctica</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>Summer visitor</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>